<commit_message>
add pom files, add correaltion graphes
</commit_message>
<xml_diff>
--- a/Project 4 Apache Common Configuration/Correlation Analysis/Correlation12&6.xlsx
+++ b/Project 4 Apache Common Configuration/Correlation Analysis/Correlation12&6.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -21,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="165">
   <si>
     <t xml:space="preserve">Version</t>
   </si>
@@ -35,10 +38,16 @@
     <t xml:space="preserve">Defect density</t>
   </si>
   <si>
-    <t xml:space="preserve">Branch &amp; Defect Density Correlation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Statement &amp; Defect Density Correlation</t>
+    <t xml:space="preserve">Branch &amp; Defect Density Correlation(Pearson)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statement &amp; Defect Density Correlation(Pearson)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch &amp; Defect Density Correlation(Spearman)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statement &amp; Defect Density Correlation(Spearman)</t>
   </si>
   <si>
     <t xml:space="preserve">2.0</t>
@@ -737,7 +746,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -938,11 +947,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="37224794"/>
-        <c:axId val="57853743"/>
+        <c:axId val="83549398"/>
+        <c:axId val="62699978"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37224794"/>
+        <c:axId val="83549398"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -998,12 +1007,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57853743"/>
+        <c:crossAx val="62699978"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57853743"/>
+        <c:axId val="62699978"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1059,7 +1068,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37224794"/>
+        <c:crossAx val="83549398"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1086,7 +1095,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1287,11 +1296,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="39997132"/>
-        <c:axId val="5067799"/>
+        <c:axId val="10035190"/>
+        <c:axId val="41691654"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39997132"/>
+        <c:axId val="10035190"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1347,12 +1356,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5067799"/>
+        <c:crossAx val="41691654"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="5067799"/>
+        <c:axId val="41691654"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1408,7 +1417,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39997132"/>
+        <c:crossAx val="10035190"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1442,13 +1451,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>100080</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>223920</xdr:colOff>
+      <xdr:colOff>223200</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>147960</xdr:rowOff>
+      <xdr:rowOff>147600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1456,8 +1465,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="100080" y="1964520"/>
-        <a:ext cx="5757840" cy="3238560"/>
+        <a:off x="100080" y="2143080"/>
+        <a:ext cx="5757120" cy="3237840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1470,15 +1479,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>779760</xdr:colOff>
+      <xdr:colOff>780120</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>15480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>12960</xdr:colOff>
+      <xdr:colOff>12600</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>2160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1486,8 +1495,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6413760" y="1981800"/>
-        <a:ext cx="5758560" cy="3238560"/>
+        <a:off x="6414120" y="2160360"/>
+        <a:ext cx="5757840" cy="3237840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1500,18 +1509,31 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.88"/>
@@ -1566,8 +1588,32 @@
         <f aca="false">PEARSON(C2:C8,D2:D8)</f>
         <v>0.6000434903449</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(B2,B$2:B$8,1)</f>
+        <v>7</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(C2,C$2:C$8,1)</f>
+        <v>4</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(D2,D$2:D$8,1)</f>
+        <v>2</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <f aca="false">H2-J2</f>
+        <v>5</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <f aca="false">K2^2</f>
+        <v>25</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <f aca="false">I2-[1]Sheet1!P16</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2.5</v>
       </c>
@@ -1580,7 +1626,36 @@
       <c r="D3" s="4" t="n">
         <v>1.44E-005</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(B3,B$2:B$8,1)</f>
+        <v>6</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(C3,C$2:C$8,1)</f>
+        <v>4</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(D3,D$2:D$8,1)</f>
+        <v>4</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <f aca="false">H3-J3</f>
+        <v>2</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <f aca="false">K3^2</f>
+        <v>4</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <f aca="false">I3-[1]Sheet1!P17</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -1595,6 +1670,37 @@
       <c r="D4" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="E4" s="0" t="n">
+        <v>-0.428571429</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">PEARSON(I2:I8,J2:J8)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(B4,B$2:B$8,1)</f>
+        <v>4</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(C4,C$2:C$8,1)</f>
+        <v>4</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(D4,D$2:D$8,1)</f>
+        <v>2</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <f aca="false">H4-J4</f>
+        <v>2</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <f aca="false">K4^2</f>
+        <v>4</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <f aca="false">I4-[1]Sheet1!P18</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -1609,6 +1715,30 @@
       <c r="D5" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(B5,B$2:B$8,1)</f>
+        <v>3</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(C5,C$2:C$8,1)</f>
+        <v>2</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(D5,D$2:D$8,1)</f>
+        <v>2</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <f aca="false">H5-J5</f>
+        <v>1</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <f aca="false">K5^2</f>
+        <v>1</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <f aca="false">I5-[1]Sheet1!P19</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1623,7 +1753,30 @@
       <c r="D6" s="4" t="n">
         <v>8.75E-005</v>
       </c>
-      <c r="K6" s="4"/>
+      <c r="H6" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(B6,B$2:B$8,1)</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(C6,C$2:C$8,1)</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(D6,D$2:D$8,1)</f>
+        <v>5</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <f aca="false">H6-J6</f>
+        <v>-3</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <f aca="false">K6^2</f>
+        <v>9</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <f aca="false">I6-[1]Sheet1!P20</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1638,11 +1791,34 @@
       <c r="D7" s="4" t="n">
         <v>8.85E-005</v>
       </c>
-      <c r="K7" s="4"/>
+      <c r="H7" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(B7,B$2:B$8,1)</f>
+        <v>5</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(C7,C$2:C$8,1)</f>
+        <v>7</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(D7,D$2:D$8,1)</f>
+        <v>6</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <f aca="false">H7-J7</f>
+        <v>-1</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <f aca="false">K7^2</f>
+        <v>1</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <f aca="false">I7-[1]Sheet1!P21</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.8317</v>
@@ -1653,10 +1829,63 @@
       <c r="D8" s="4" t="n">
         <v>0.00015</v>
       </c>
-      <c r="K8" s="4"/>
+      <c r="H8" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(B8,B$2:B$8,1)</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(C8,C$2:C$8,1)</f>
+        <v>6</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <f aca="false">_xlfn.RANK.AVG(D8,D$2:D$8,1)</f>
+        <v>7</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <f aca="false">H8-J8</f>
+        <v>-6</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <f aca="false">K8^2</f>
+        <v>36</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <f aca="false">I8-[1]Sheet1!P22</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D9" s="4"/>
+      <c r="L9" s="0" t="n">
+        <f aca="false">SUM(L2:L8)</f>
+        <v>80</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <f aca="false">SUM(M2:M8)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L10" s="0" t="n">
+        <f aca="false">1-L9*6/(7^3-7)</f>
+        <v>-0.428571428571429</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <f aca="false">1-M9*6/(7^3-7)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J11" s="0" t="n">
+        <f aca="false">PEARSON(H2:H8,J2:J8)</f>
+        <v>-0.481812055829716</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J13" s="0" t="n">
+        <f aca="false">PEARSON(I2:I8,J2:J8)</f>
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1681,1427 +1910,1427 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8"/>
       <c r="B2" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8"/>
       <c r="B3" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8"/>
       <c r="B4" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8"/>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
       <c r="B6" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8"/>
       <c r="B8" s="6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="7" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
       <c r="B9" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8"/>
       <c r="B10" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8"/>
       <c r="B11" s="6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8"/>
       <c r="B12" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8"/>
       <c r="B13" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8"/>
       <c r="B14" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
       <c r="B15" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8"/>
       <c r="B16" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8"/>
       <c r="B17" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="7" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8"/>
       <c r="B18" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="7" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
       <c r="B19" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8"/>
       <c r="B20" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
       <c r="B21" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="7" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8"/>
       <c r="B22" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8"/>
       <c r="B23" s="6" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
       <c r="B24" s="6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8"/>
       <c r="B25" s="6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8"/>
       <c r="B26" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8"/>
       <c r="B27" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8"/>
       <c r="B28" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8"/>
       <c r="B29" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8"/>
       <c r="B30" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
       <c r="B31" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="8"/>
       <c r="B32" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="8"/>
       <c r="B33" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8"/>
       <c r="B34" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="8"/>
       <c r="B35" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8"/>
       <c r="B36" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8"/>
       <c r="B37" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="8"/>
       <c r="B38" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="8"/>
       <c r="B39" s="6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8"/>
       <c r="B40" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="7" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8"/>
       <c r="B41" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="7" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8"/>
       <c r="B42" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="7" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8"/>
       <c r="B43" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8"/>
       <c r="B44" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8"/>
       <c r="B45" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="7" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8"/>
       <c r="B46" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8"/>
       <c r="B47" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="7" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8"/>
       <c r="B48" s="6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8"/>
       <c r="B49" s="6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C49" s="8"/>
       <c r="D49" s="7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8"/>
       <c r="B50" s="6" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C50" s="8"/>
       <c r="D50" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8"/>
       <c r="B51" s="6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C51" s="8"/>
       <c r="D51" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="8"/>
       <c r="B52" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C52" s="8"/>
       <c r="D52" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="8"/>
       <c r="B53" s="6" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C53" s="8"/>
       <c r="D53" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8"/>
       <c r="B54" s="6" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C54" s="8"/>
       <c r="D54" s="7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8"/>
       <c r="B55" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C55" s="8"/>
       <c r="D55" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8"/>
       <c r="B56" s="6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C56" s="8"/>
       <c r="D56" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8"/>
       <c r="B57" s="6" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C57" s="8"/>
       <c r="D57" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8"/>
       <c r="B58" s="6" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C58" s="8"/>
       <c r="D58" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8"/>
       <c r="B59" s="6" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C59" s="8"/>
       <c r="D59" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8"/>
       <c r="B60" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C60" s="8"/>
       <c r="D60" s="7" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8"/>
       <c r="B61" s="6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C61" s="8"/>
       <c r="D61" s="7" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="8"/>
       <c r="B62" s="6" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C62" s="8"/>
       <c r="D62" s="7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="8"/>
       <c r="B63" s="6" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C63" s="8"/>
       <c r="D63" s="7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="8"/>
       <c r="B64" s="6" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C64" s="8"/>
       <c r="D64" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="8"/>
       <c r="B65" s="6" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C65" s="8"/>
       <c r="D65" s="7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="8"/>
       <c r="B66" s="6" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="7" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="8"/>
       <c r="B67" s="6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C67" s="8"/>
       <c r="D67" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="8"/>
       <c r="B68" s="6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C68" s="8"/>
       <c r="D68" s="7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="8"/>
       <c r="B69" s="6" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C69" s="8"/>
       <c r="D69" s="7" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="8"/>
       <c r="B70" s="6" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C70" s="8"/>
       <c r="D70" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="8"/>
       <c r="B71" s="6" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="7" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="8"/>
       <c r="B72" s="6" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C72" s="8"/>
       <c r="D72" s="7" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="8"/>
       <c r="B73" s="6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C73" s="8"/>
       <c r="D73" s="7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="8"/>
       <c r="B74" s="6" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="7" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="8"/>
       <c r="B75" s="6" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="7" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>